<commit_message>
Updated Draft Progress Report 1
</commit_message>
<xml_diff>
--- a/ProjectManagement/task_calendar.xlsx
+++ b/ProjectManagement/task_calendar.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="21405"/>
-  <workbookPr filterPrivacy="1" autoCompressPictures="0"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+  <workbookPr filterPrivacy="1" autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="20" yWindow="0" windowWidth="28560" windowHeight="17440"/>
+    <workbookView xWindow="15" yWindow="0" windowWidth="28560" windowHeight="17445"/>
   </bookViews>
   <sheets>
     <sheet name="Top Level" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="63">
   <si>
     <t>PROJECT PHASE</t>
   </si>
@@ -197,6 +197,18 @@
   </si>
   <si>
     <t>Per</t>
+  </si>
+  <si>
+    <t>Android Task 5</t>
+  </si>
+  <si>
+    <t>Android Task 6</t>
+  </si>
+  <si>
+    <t>Android Task 7</t>
+  </si>
+  <si>
+    <t>Thomas, Mohammad &amp; Jonas</t>
   </si>
 </sst>
 </file>
@@ -266,12 +278,30 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -463,7 +493,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
@@ -500,9 +530,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -510,6 +537,26 @@
     </xf>
     <xf numFmtId="14" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
       <protection locked="0"/>
     </xf>
   </cellXfs>
@@ -978,41 +1025,41 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F52"/>
+  <dimension ref="A1:F55"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="F27" sqref="A1:F27"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.83203125" customWidth="1"/>
+    <col min="1" max="1" width="21.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="27" customWidth="1"/>
-    <col min="3" max="3" width="22.83203125" customWidth="1"/>
-    <col min="4" max="4" width="24.83203125" customWidth="1"/>
-    <col min="5" max="5" width="10.5" customWidth="1"/>
-    <col min="6" max="6" width="24.6640625" customWidth="1"/>
+    <col min="3" max="3" width="22.85546875" customWidth="1"/>
+    <col min="4" max="4" width="24.85546875" customWidth="1"/>
+    <col min="5" max="5" width="10.42578125" customWidth="1"/>
+    <col min="6" max="6" width="24.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="25">
-      <c r="A1" s="21"/>
-      <c r="B1" s="21"/>
-      <c r="C1" s="22" t="s">
+    <row r="1" spans="1:6" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A1" s="20"/>
+      <c r="B1" s="20"/>
+      <c r="C1" s="21" t="s">
         <v>47</v>
       </c>
-      <c r="D1" s="21"/>
-      <c r="E1" s="21"/>
-      <c r="F1" s="21"/>
-    </row>
-    <row r="2" spans="1:6">
-      <c r="A2" s="21"/>
-      <c r="B2" s="21"/>
-      <c r="C2" s="21"/>
-      <c r="D2" s="21"/>
-      <c r="E2" s="21"/>
-      <c r="F2" s="21"/>
-    </row>
-    <row r="3" spans="1:6" ht="15">
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="20"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="20"/>
+      <c r="B2" s="20"/>
+      <c r="C2" s="20"/>
+      <c r="D2" s="20"/>
+      <c r="E2" s="20"/>
+      <c r="F2" s="20"/>
+    </row>
+    <row r="3" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>0</v>
       </c>
@@ -1032,11 +1079,11 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
-      <c r="A4" s="20" t="s">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="24" t="s">
         <v>16</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="25" t="s">
         <v>2</v>
       </c>
       <c r="C4" s="1"/>
@@ -1048,9 +1095,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
-      <c r="A5" s="20"/>
-      <c r="B5" s="1" t="s">
+    <row r="5" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A5" s="24"/>
+      <c r="B5" s="30" t="s">
         <v>4</v>
       </c>
       <c r="C5" s="1"/>
@@ -1062,9 +1109,9 @@
         <v>46</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
-      <c r="A6" s="20"/>
-      <c r="B6" s="1" t="s">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="24"/>
+      <c r="B6" s="25" t="s">
         <v>12</v>
       </c>
       <c r="C6" s="1"/>
@@ -1076,9 +1123,9 @@
         <v>45</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
-      <c r="A7" s="20"/>
-      <c r="B7" s="8" t="s">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="24"/>
+      <c r="B7" s="26" t="s">
         <v>5</v>
       </c>
       <c r="C7" s="8"/>
@@ -1092,10 +1139,10 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
-      <c r="A8" s="20"/>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="24"/>
       <c r="B8" s="8"/>
-      <c r="C8" s="1" t="s">
+      <c r="C8" s="25" t="s">
         <v>7</v>
       </c>
       <c r="D8" s="8"/>
@@ -1106,10 +1153,10 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
-      <c r="A9" s="20"/>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="24"/>
       <c r="B9" s="9"/>
-      <c r="C9" s="9" t="s">
+      <c r="C9" s="27" t="s">
         <v>29</v>
       </c>
       <c r="D9" s="2"/>
@@ -1120,9 +1167,9 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
-      <c r="A10" s="20"/>
-      <c r="B10" s="9" t="s">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="24"/>
+      <c r="B10" s="27" t="s">
         <v>39</v>
       </c>
       <c r="C10" s="9"/>
@@ -1134,9 +1181,9 @@
         <v>36</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
-      <c r="A11" s="20"/>
-      <c r="B11" s="9" t="s">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="24"/>
+      <c r="B11" s="27" t="s">
         <v>40</v>
       </c>
       <c r="C11" s="9"/>
@@ -1148,9 +1195,9 @@
         <v>37</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
-      <c r="A12" s="20"/>
-      <c r="B12" s="9" t="s">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="24"/>
+      <c r="B12" s="27" t="s">
         <v>41</v>
       </c>
       <c r="C12" s="9"/>
@@ -1162,9 +1209,9 @@
         <v>37</v>
       </c>
     </row>
-    <row r="13" spans="1:6">
-      <c r="A13" s="20"/>
-      <c r="B13" s="9" t="s">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="24"/>
+      <c r="B13" s="27" t="s">
         <v>42</v>
       </c>
       <c r="C13" s="9"/>
@@ -1176,498 +1223,540 @@
         <v>38</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="28">
-      <c r="A14" s="20"/>
-      <c r="B14" s="9" t="s">
-        <v>44</v>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="24"/>
+      <c r="B14" s="27" t="s">
+        <v>59</v>
       </c>
       <c r="C14" s="9"/>
       <c r="D14" s="2"/>
       <c r="E14" s="4">
-        <v>42102</v>
+        <v>42103</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6">
-      <c r="A15" s="20"/>
-      <c r="B15" s="9"/>
-      <c r="C15" s="9" t="s">
-        <v>30</v>
-      </c>
+        <v>38</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="24"/>
+      <c r="B15" s="27" t="s">
+        <v>60</v>
+      </c>
+      <c r="C15" s="9"/>
       <c r="D15" s="2"/>
       <c r="E15" s="4">
-        <v>42109</v>
+        <v>42103</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6">
-      <c r="A16" s="20"/>
-      <c r="B16" s="9"/>
-      <c r="C16" s="9" t="s">
-        <v>55</v>
-      </c>
+        <v>38</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="24"/>
+      <c r="B16" s="29" t="s">
+        <v>61</v>
+      </c>
+      <c r="C16" s="9"/>
       <c r="D16" s="2"/>
-      <c r="E16" s="4">
-        <v>42109</v>
+      <c r="E16" s="15">
+        <v>42108</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6">
-      <c r="A17" s="20"/>
-      <c r="B17" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="C17" s="3"/>
+        <v>62</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A17" s="24"/>
+      <c r="B17" s="28" t="s">
+        <v>44</v>
+      </c>
+      <c r="C17" s="9"/>
       <c r="D17" s="2"/>
       <c r="E17" s="4">
-        <v>42114</v>
+        <v>42102</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6">
-      <c r="A18" s="20"/>
-      <c r="B18" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C18" s="3"/>
+        <v>45</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="24"/>
+      <c r="B18" s="9"/>
+      <c r="C18" s="27" t="s">
+        <v>30</v>
+      </c>
       <c r="D18" s="2"/>
       <c r="E18" s="4">
+        <v>42109</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="24"/>
+      <c r="B19" s="9"/>
+      <c r="C19" s="27" t="s">
+        <v>55</v>
+      </c>
+      <c r="D19" s="2"/>
+      <c r="E19" s="4">
+        <v>42109</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" s="24"/>
+      <c r="B20" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C20" s="3"/>
+      <c r="D20" s="2"/>
+      <c r="E20" s="4">
+        <v>42114</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="24"/>
+      <c r="B21" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C21" s="3"/>
+      <c r="D21" s="2"/>
+      <c r="E21" s="4">
         <v>42115</v>
       </c>
-      <c r="F18" s="2" t="s">
+      <c r="F21" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="19" spans="1:6">
-      <c r="A19" s="20"/>
-      <c r="B19" s="8"/>
-      <c r="C19" s="3" t="s">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" s="24"/>
+      <c r="B22" s="8"/>
+      <c r="C22" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D19" s="3"/>
-      <c r="E19" s="4">
-        <v>42116</v>
-      </c>
-      <c r="F19" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6">
-      <c r="A20" s="20"/>
-      <c r="B20" s="8"/>
-      <c r="C20" s="3"/>
-      <c r="D20" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E20" s="23" t="s">
-        <v>57</v>
-      </c>
-      <c r="F20" s="2" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6">
-      <c r="A21" s="20"/>
-      <c r="B21" s="9"/>
-      <c r="C21" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="D21" s="4"/>
-      <c r="E21" s="4">
-        <v>42116</v>
-      </c>
-      <c r="F21" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6">
-      <c r="A22" s="20"/>
-      <c r="B22" s="9"/>
-      <c r="C22" s="9" t="s">
-        <v>56</v>
-      </c>
-      <c r="D22" s="4"/>
+      <c r="D22" s="3"/>
       <c r="E22" s="4">
         <v>42116</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6">
-      <c r="A23" s="20"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" s="24"/>
       <c r="B23" s="8"/>
-      <c r="C23" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D23" s="3"/>
-      <c r="E23" s="5">
-        <v>42123</v>
+      <c r="C23" s="3"/>
+      <c r="D23" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E23" s="22" t="s">
+        <v>57</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6">
-      <c r="A24" s="20"/>
-      <c r="B24" s="8"/>
-      <c r="C24" s="3"/>
-      <c r="D24" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="E24" s="24" t="s">
-        <v>57</v>
+        <v>58</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" s="24"/>
+      <c r="B24" s="9"/>
+      <c r="C24" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="D24" s="4"/>
+      <c r="E24" s="4">
+        <v>42116</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6">
-      <c r="A25" s="20"/>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" s="24"/>
       <c r="B25" s="9"/>
       <c r="C25" s="9" t="s">
-        <v>49</v>
-      </c>
-      <c r="D25" s="5"/>
-      <c r="E25" s="5">
-        <v>42123</v>
+        <v>56</v>
+      </c>
+      <c r="D25" s="4"/>
+      <c r="E25" s="4">
+        <v>42116</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6">
-      <c r="A26" s="20"/>
-      <c r="B26" s="9"/>
-      <c r="C26" s="9" t="s">
-        <v>50</v>
-      </c>
-      <c r="D26" s="5"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" s="24"/>
+      <c r="B26" s="8"/>
+      <c r="C26" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D26" s="3"/>
       <c r="E26" s="5">
         <v>42123</v>
       </c>
       <c r="F26" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" s="24"/>
+      <c r="B27" s="8"/>
+      <c r="C27" s="3"/>
+      <c r="D27" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E27" s="23" t="s">
+        <v>57</v>
+      </c>
+      <c r="F27" s="2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" s="24"/>
+      <c r="B28" s="9"/>
+      <c r="C28" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="D28" s="5"/>
+      <c r="E28" s="5">
+        <v>42123</v>
+      </c>
+      <c r="F28" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" s="24"/>
+      <c r="B29" s="9"/>
+      <c r="C29" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="D29" s="5"/>
+      <c r="E29" s="5">
+        <v>42123</v>
+      </c>
+      <c r="F29" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="27" spans="1:6" ht="25">
-      <c r="A27" s="20"/>
-      <c r="B27" s="10" t="s">
+    <row r="30" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A30" s="24"/>
+      <c r="B30" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="C27" s="8"/>
-      <c r="D27" s="8"/>
-      <c r="E27" s="11">
+      <c r="C30" s="8"/>
+      <c r="D30" s="8"/>
+      <c r="E30" s="11">
         <v>42124</v>
       </c>
-      <c r="F27" s="2" t="s">
+      <c r="F30" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="28" spans="1:6" ht="28">
-      <c r="A28" s="20" t="s">
+    <row r="31" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A31" s="24" t="s">
         <v>17</v>
       </c>
-      <c r="B28" s="9" t="s">
+      <c r="B31" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="C28" s="9"/>
-      <c r="D28" s="8"/>
-      <c r="E28" s="11">
+      <c r="C31" s="9"/>
+      <c r="D31" s="8"/>
+      <c r="E31" s="11">
         <v>42125</v>
       </c>
-      <c r="F28" s="6" t="s">
+      <c r="F31" s="6" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="29" spans="1:6">
-      <c r="A29" s="20"/>
-      <c r="B29" s="8"/>
-      <c r="C29" s="3" t="s">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" s="24"/>
+      <c r="B32" s="8"/>
+      <c r="C32" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D29" s="3"/>
-      <c r="E29" s="5">
-        <v>42130</v>
-      </c>
-      <c r="F29" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6">
-      <c r="A30" s="20"/>
-      <c r="B30" s="8"/>
-      <c r="C30" s="3"/>
-      <c r="D30" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="E30" s="24" t="s">
-        <v>57</v>
-      </c>
-      <c r="F30" s="2" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" ht="37">
-      <c r="A31" s="20"/>
-      <c r="B31" s="8"/>
-      <c r="C31" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="D31" s="8"/>
-      <c r="E31" s="5">
-        <v>42131</v>
-      </c>
-      <c r="F31" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6">
-      <c r="A32" s="20"/>
-      <c r="B32" s="9"/>
-      <c r="C32" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="D32" s="8"/>
+      <c r="D32" s="3"/>
       <c r="E32" s="5">
         <v>42130</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6">
-      <c r="A33" s="20"/>
-      <c r="B33" s="9"/>
-      <c r="C33" s="9" t="s">
-        <v>51</v>
-      </c>
-      <c r="D33" s="8"/>
-      <c r="E33" s="5">
-        <v>42130</v>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" s="24"/>
+      <c r="B33" s="8"/>
+      <c r="C33" s="3"/>
+      <c r="D33" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E33" s="23" t="s">
+        <v>57</v>
       </c>
       <c r="F33" s="2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" ht="39" x14ac:dyDescent="0.25">
+      <c r="A34" s="24"/>
+      <c r="B34" s="8"/>
+      <c r="C34" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="D34" s="8"/>
+      <c r="E34" s="5">
+        <v>42131</v>
+      </c>
+      <c r="F34" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="34" spans="1:6">
-      <c r="A34" s="20"/>
-      <c r="B34" s="9"/>
-      <c r="C34" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="D34" s="8"/>
-      <c r="E34" s="4">
-        <v>42137</v>
-      </c>
-      <c r="F34" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6">
-      <c r="A35" s="20"/>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35" s="24"/>
       <c r="B35" s="9"/>
       <c r="C35" s="9" t="s">
-        <v>52</v>
+        <v>32</v>
       </c>
       <c r="D35" s="8"/>
-      <c r="E35" s="4">
-        <v>42137</v>
+      <c r="E35" s="5">
+        <v>42130</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" ht="37">
-      <c r="A36" s="20"/>
-      <c r="B36" s="8"/>
-      <c r="C36" s="12" t="s">
-        <v>24</v>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A36" s="24"/>
+      <c r="B36" s="9"/>
+      <c r="C36" s="9" t="s">
+        <v>51</v>
       </c>
       <c r="D36" s="8"/>
-      <c r="E36" s="4">
-        <v>42138</v>
+      <c r="E36" s="5">
+        <v>42130</v>
       </c>
       <c r="F36" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="37" spans="1:6">
-      <c r="A37" s="20"/>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A37" s="24"/>
       <c r="B37" s="9"/>
       <c r="C37" s="9" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D37" s="8"/>
       <c r="E37" s="4">
-        <v>42144</v>
+        <v>42137</v>
       </c>
       <c r="F37" s="2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="38" spans="1:6">
-      <c r="A38" s="20"/>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A38" s="24"/>
       <c r="B38" s="9"/>
       <c r="C38" s="9" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D38" s="8"/>
       <c r="E38" s="4">
-        <v>42144</v>
+        <v>42137</v>
       </c>
       <c r="F38" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="39" spans="1:6">
-      <c r="A39" s="20"/>
-      <c r="B39" s="9"/>
-      <c r="C39" s="9" t="s">
-        <v>54</v>
+    <row r="39" spans="1:6" ht="39" x14ac:dyDescent="0.25">
+      <c r="A39" s="24"/>
+      <c r="B39" s="8"/>
+      <c r="C39" s="12" t="s">
+        <v>24</v>
       </c>
       <c r="D39" s="8"/>
       <c r="E39" s="4">
-        <v>42151</v>
+        <v>42138</v>
       </c>
       <c r="F39" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="40" spans="1:6" ht="28">
-      <c r="A40" s="20"/>
-      <c r="B40" s="8"/>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A40" s="24"/>
+      <c r="B40" s="9"/>
       <c r="C40" s="9" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
       <c r="D40" s="8"/>
       <c r="E40" s="4">
-        <v>42151</v>
+        <v>42144</v>
       </c>
       <c r="F40" s="2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="41" spans="1:6" ht="15" customHeight="1">
-      <c r="A41" s="20"/>
-      <c r="B41" s="8"/>
-      <c r="C41" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D41" s="1"/>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A41" s="24"/>
+      <c r="B41" s="9"/>
+      <c r="C41" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="D41" s="8"/>
       <c r="E41" s="4">
-        <v>42152</v>
+        <v>42144</v>
       </c>
       <c r="F41" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" ht="15" customHeight="1">
-      <c r="A42" s="20"/>
-      <c r="B42" s="8"/>
-      <c r="C42" s="1"/>
-      <c r="D42" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="E42" s="23" t="s">
-        <v>57</v>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A42" s="24"/>
+      <c r="B42" s="9"/>
+      <c r="C42" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="D42" s="8"/>
+      <c r="E42" s="4">
+        <v>42151</v>
       </c>
       <c r="F42" s="2" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" ht="15" customHeight="1">
-      <c r="A43" s="20">
-        <v>2</v>
-      </c>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A43" s="24"/>
       <c r="B43" s="8"/>
-      <c r="C43" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D43" s="1"/>
+      <c r="C43" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="D43" s="8"/>
       <c r="E43" s="4">
-        <v>42153</v>
+        <v>42151</v>
       </c>
       <c r="F43" s="2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="44" spans="1:6" ht="15" customHeight="1">
-      <c r="A44" s="20"/>
+    <row r="44" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="24"/>
       <c r="B44" s="8"/>
-      <c r="C44" s="13" t="s">
+      <c r="C44" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D44" s="1"/>
+      <c r="E44" s="4">
+        <v>42152</v>
+      </c>
+      <c r="F44" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="24"/>
+      <c r="B45" s="8"/>
+      <c r="C45" s="1"/>
+      <c r="D45" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E45" s="22" t="s">
+        <v>57</v>
+      </c>
+      <c r="F45" s="2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="24">
+        <v>2</v>
+      </c>
+      <c r="B46" s="8"/>
+      <c r="C46" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D46" s="1"/>
+      <c r="E46" s="4">
+        <v>42153</v>
+      </c>
+      <c r="F46" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="24"/>
+      <c r="B47" s="8"/>
+      <c r="C47" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="D44" s="2"/>
-      <c r="E44" s="4">
+      <c r="D47" s="2"/>
+      <c r="E47" s="4">
         <v>42156</v>
       </c>
-      <c r="F44" s="2" t="s">
+      <c r="F47" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="45" spans="1:6" ht="15" customHeight="1">
-      <c r="A45" s="16"/>
-      <c r="B45" s="17"/>
-      <c r="C45" s="17"/>
-      <c r="D45" s="18"/>
-      <c r="E45" s="14"/>
-      <c r="F45" s="18"/>
-    </row>
-    <row r="46" spans="1:6">
-      <c r="A46" s="16"/>
-      <c r="B46" s="19"/>
-      <c r="C46" s="19"/>
-      <c r="D46" s="18"/>
-      <c r="E46" s="14"/>
-      <c r="F46" s="18"/>
-    </row>
-    <row r="47" spans="1:6">
-      <c r="A47" s="16"/>
-      <c r="B47" s="18"/>
-      <c r="C47" s="18"/>
-      <c r="D47" s="19"/>
-      <c r="E47" s="14"/>
-      <c r="F47" s="18"/>
-    </row>
-    <row r="48" spans="1:6">
+    <row r="48" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="16"/>
-      <c r="B48" s="19"/>
-      <c r="C48" s="19"/>
+      <c r="B48" s="17"/>
+      <c r="C48" s="17"/>
       <c r="D48" s="18"/>
       <c r="E48" s="14"/>
       <c r="F48" s="18"/>
     </row>
-    <row r="49" spans="5:5">
-      <c r="E49" s="15"/>
-    </row>
-    <row r="50" spans="5:5">
-      <c r="E50" s="15"/>
-    </row>
-    <row r="51" spans="5:5">
-      <c r="E51" s="15"/>
-    </row>
-    <row r="52" spans="5:5">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A49" s="16"/>
+      <c r="B49" s="19"/>
+      <c r="C49" s="19"/>
+      <c r="D49" s="18"/>
+      <c r="E49" s="14"/>
+      <c r="F49" s="18"/>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A50" s="16"/>
+      <c r="B50" s="18"/>
+      <c r="C50" s="18"/>
+      <c r="D50" s="19"/>
+      <c r="E50" s="14"/>
+      <c r="F50" s="18"/>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A51" s="16"/>
+      <c r="B51" s="19"/>
+      <c r="C51" s="19"/>
+      <c r="D51" s="18"/>
+      <c r="E51" s="14"/>
+      <c r="F51" s="18"/>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E52" s="15"/>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E53" s="15"/>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E54" s="15"/>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E55" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="A4:A27"/>
-    <mergeCell ref="A28:A44"/>
+    <mergeCell ref="A4:A30"/>
+    <mergeCell ref="A31:A47"/>
   </mergeCells>
   <phoneticPr fontId="8" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="67" orientation="landscape" horizontalDpi="4294967293" verticalDpi="4294967293"/>
   <rowBreaks count="1" manualBreakCount="1">
-    <brk id="44" max="16383" man="1"/>
+    <brk id="47" max="16383" man="1"/>
   </rowBreaks>
   <colBreaks count="1" manualBreakCount="1">
     <brk id="7" max="1048575" man="1"/>
@@ -1686,7 +1775,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>

</xml_diff>

<commit_message>
Revert "Updated Draft Progress Report 1"
This reverts commit c765f6d6032cd07b8685f07a1f0c49a90ffcac53.
</commit_message>
<xml_diff>
--- a/ProjectManagement/task_calendar.xlsx
+++ b/ProjectManagement/task_calendar.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" autoCompressPictures="0" defaultThemeVersion="124226"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="21405"/>
+  <workbookPr filterPrivacy="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="15" yWindow="0" windowWidth="28560" windowHeight="17445"/>
+    <workbookView xWindow="20" yWindow="0" windowWidth="28560" windowHeight="17440"/>
   </bookViews>
   <sheets>
     <sheet name="Top Level" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="59">
   <si>
     <t>PROJECT PHASE</t>
   </si>
@@ -197,18 +197,6 @@
   </si>
   <si>
     <t>Per</t>
-  </si>
-  <si>
-    <t>Android Task 5</t>
-  </si>
-  <si>
-    <t>Android Task 6</t>
-  </si>
-  <si>
-    <t>Android Task 7</t>
-  </si>
-  <si>
-    <t>Thomas, Mohammad &amp; Jonas</t>
   </si>
 </sst>
 </file>
@@ -278,30 +266,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF00B050"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -493,7 +463,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
@@ -530,6 +500,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -537,26 +510,6 @@
     </xf>
     <xf numFmtId="14" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment wrapText="1"/>
       <protection locked="0"/>
     </xf>
   </cellXfs>
@@ -1025,41 +978,41 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F55"/>
+  <dimension ref="A1:F52"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="F27" sqref="A1:F27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="21.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.83203125" customWidth="1"/>
     <col min="2" max="2" width="27" customWidth="1"/>
-    <col min="3" max="3" width="22.85546875" customWidth="1"/>
-    <col min="4" max="4" width="24.85546875" customWidth="1"/>
-    <col min="5" max="5" width="10.42578125" customWidth="1"/>
-    <col min="6" max="6" width="24.7109375" customWidth="1"/>
+    <col min="3" max="3" width="22.83203125" customWidth="1"/>
+    <col min="4" max="4" width="24.83203125" customWidth="1"/>
+    <col min="5" max="5" width="10.5" customWidth="1"/>
+    <col min="6" max="6" width="24.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A1" s="20"/>
-      <c r="B1" s="20"/>
-      <c r="C1" s="21" t="s">
+    <row r="1" spans="1:6" ht="25">
+      <c r="A1" s="21"/>
+      <c r="B1" s="21"/>
+      <c r="C1" s="22" t="s">
         <v>47</v>
       </c>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
-      <c r="F1" s="20"/>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="20"/>
-      <c r="B2" s="20"/>
-      <c r="C2" s="20"/>
-      <c r="D2" s="20"/>
-      <c r="E2" s="20"/>
-      <c r="F2" s="20"/>
-    </row>
-    <row r="3" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D1" s="21"/>
+      <c r="E1" s="21"/>
+      <c r="F1" s="21"/>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="21"/>
+      <c r="B2" s="21"/>
+      <c r="C2" s="21"/>
+      <c r="D2" s="21"/>
+      <c r="E2" s="21"/>
+      <c r="F2" s="21"/>
+    </row>
+    <row r="3" spans="1:6" ht="15">
       <c r="A3" s="7" t="s">
         <v>0</v>
       </c>
@@ -1079,11 +1032,11 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="24" t="s">
+    <row r="4" spans="1:6">
+      <c r="A4" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="B4" s="25" t="s">
+      <c r="B4" s="1" t="s">
         <v>2</v>
       </c>
       <c r="C4" s="1"/>
@@ -1095,9 +1048,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A5" s="24"/>
-      <c r="B5" s="30" t="s">
+    <row r="5" spans="1:6">
+      <c r="A5" s="20"/>
+      <c r="B5" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C5" s="1"/>
@@ -1109,9 +1062,9 @@
         <v>46</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="24"/>
-      <c r="B6" s="25" t="s">
+    <row r="6" spans="1:6">
+      <c r="A6" s="20"/>
+      <c r="B6" s="1" t="s">
         <v>12</v>
       </c>
       <c r="C6" s="1"/>
@@ -1123,9 +1076,9 @@
         <v>45</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="24"/>
-      <c r="B7" s="26" t="s">
+    <row r="7" spans="1:6">
+      <c r="A7" s="20"/>
+      <c r="B7" s="8" t="s">
         <v>5</v>
       </c>
       <c r="C7" s="8"/>
@@ -1139,10 +1092,10 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="24"/>
+    <row r="8" spans="1:6">
+      <c r="A8" s="20"/>
       <c r="B8" s="8"/>
-      <c r="C8" s="25" t="s">
+      <c r="C8" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D8" s="8"/>
@@ -1153,10 +1106,10 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="24"/>
+    <row r="9" spans="1:6">
+      <c r="A9" s="20"/>
       <c r="B9" s="9"/>
-      <c r="C9" s="27" t="s">
+      <c r="C9" s="9" t="s">
         <v>29</v>
       </c>
       <c r="D9" s="2"/>
@@ -1167,9 +1120,9 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="24"/>
-      <c r="B10" s="27" t="s">
+    <row r="10" spans="1:6">
+      <c r="A10" s="20"/>
+      <c r="B10" s="9" t="s">
         <v>39</v>
       </c>
       <c r="C10" s="9"/>
@@ -1181,9 +1134,9 @@
         <v>36</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="24"/>
-      <c r="B11" s="27" t="s">
+    <row r="11" spans="1:6">
+      <c r="A11" s="20"/>
+      <c r="B11" s="9" t="s">
         <v>40</v>
       </c>
       <c r="C11" s="9"/>
@@ -1195,9 +1148,9 @@
         <v>37</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="24"/>
-      <c r="B12" s="27" t="s">
+    <row r="12" spans="1:6">
+      <c r="A12" s="20"/>
+      <c r="B12" s="9" t="s">
         <v>41</v>
       </c>
       <c r="C12" s="9"/>
@@ -1209,9 +1162,9 @@
         <v>37</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="24"/>
-      <c r="B13" s="27" t="s">
+    <row r="13" spans="1:6">
+      <c r="A13" s="20"/>
+      <c r="B13" s="9" t="s">
         <v>42</v>
       </c>
       <c r="C13" s="9"/>
@@ -1223,540 +1176,498 @@
         <v>38</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="24"/>
-      <c r="B14" s="27" t="s">
-        <v>59</v>
+    <row r="14" spans="1:6" ht="28">
+      <c r="A14" s="20"/>
+      <c r="B14" s="9" t="s">
+        <v>44</v>
       </c>
       <c r="C14" s="9"/>
       <c r="D14" s="2"/>
       <c r="E14" s="4">
-        <v>42103</v>
+        <v>42102</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="24"/>
-      <c r="B15" s="27" t="s">
-        <v>60</v>
-      </c>
-      <c r="C15" s="9"/>
+        <v>45</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15" s="20"/>
+      <c r="B15" s="9"/>
+      <c r="C15" s="9" t="s">
+        <v>30</v>
+      </c>
       <c r="D15" s="2"/>
       <c r="E15" s="4">
-        <v>42103</v>
+        <v>42109</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="24"/>
-      <c r="B16" s="29" t="s">
-        <v>61</v>
-      </c>
-      <c r="C16" s="9"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16" s="20"/>
+      <c r="B16" s="9"/>
+      <c r="C16" s="9" t="s">
+        <v>55</v>
+      </c>
       <c r="D16" s="2"/>
-      <c r="E16" s="15">
-        <v>42108</v>
+      <c r="E16" s="4">
+        <v>42109</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A17" s="24"/>
-      <c r="B17" s="28" t="s">
-        <v>44</v>
-      </c>
-      <c r="C17" s="9"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="A17" s="20"/>
+      <c r="B17" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C17" s="3"/>
       <c r="D17" s="2"/>
       <c r="E17" s="4">
-        <v>42102</v>
+        <v>42114</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="24"/>
-      <c r="B18" s="9"/>
-      <c r="C18" s="27" t="s">
-        <v>30</v>
-      </c>
+        <v>46</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
+      <c r="A18" s="20"/>
+      <c r="B18" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C18" s="3"/>
       <c r="D18" s="2"/>
       <c r="E18" s="4">
-        <v>42109</v>
+        <v>42115</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="24"/>
-      <c r="B19" s="9"/>
-      <c r="C19" s="27" t="s">
-        <v>55</v>
-      </c>
-      <c r="D19" s="2"/>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
+      <c r="A19" s="20"/>
+      <c r="B19" s="8"/>
+      <c r="C19" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D19" s="3"/>
       <c r="E19" s="4">
-        <v>42109</v>
+        <v>42116</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="24"/>
-      <c r="B20" s="3" t="s">
-        <v>43</v>
-      </c>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
+      <c r="A20" s="20"/>
+      <c r="B20" s="8"/>
       <c r="C20" s="3"/>
-      <c r="D20" s="2"/>
-      <c r="E20" s="4">
-        <v>42114</v>
+      <c r="D20" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E20" s="23" t="s">
+        <v>57</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="24"/>
-      <c r="B21" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C21" s="3"/>
-      <c r="D21" s="2"/>
+        <v>58</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
+      <c r="A21" s="20"/>
+      <c r="B21" s="9"/>
+      <c r="C21" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="D21" s="4"/>
       <c r="E21" s="4">
-        <v>42115</v>
+        <v>42116</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="24"/>
-      <c r="B22" s="8"/>
-      <c r="C22" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D22" s="3"/>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6">
+      <c r="A22" s="20"/>
+      <c r="B22" s="9"/>
+      <c r="C22" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="D22" s="4"/>
       <c r="E22" s="4">
         <v>42116</v>
       </c>
       <c r="F22" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6">
+      <c r="A23" s="20"/>
+      <c r="B23" s="8"/>
+      <c r="C23" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D23" s="3"/>
+      <c r="E23" s="5">
+        <v>42123</v>
+      </c>
+      <c r="F23" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="24"/>
-      <c r="B23" s="8"/>
-      <c r="C23" s="3"/>
-      <c r="D23" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E23" s="22" t="s">
+    <row r="24" spans="1:6">
+      <c r="A24" s="20"/>
+      <c r="B24" s="8"/>
+      <c r="C24" s="3"/>
+      <c r="D24" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E24" s="24" t="s">
         <v>57</v>
       </c>
-      <c r="F23" s="2" t="s">
+      <c r="F24" s="2" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="24"/>
-      <c r="B24" s="9"/>
-      <c r="C24" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="D24" s="4"/>
-      <c r="E24" s="4">
-        <v>42116</v>
-      </c>
-      <c r="F24" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" s="24"/>
+    <row r="25" spans="1:6">
+      <c r="A25" s="20"/>
       <c r="B25" s="9"/>
       <c r="C25" s="9" t="s">
-        <v>56</v>
-      </c>
-      <c r="D25" s="4"/>
-      <c r="E25" s="4">
-        <v>42116</v>
+        <v>49</v>
+      </c>
+      <c r="D25" s="5"/>
+      <c r="E25" s="5">
+        <v>42123</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" s="24"/>
-      <c r="B26" s="8"/>
-      <c r="C26" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D26" s="3"/>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6">
+      <c r="A26" s="20"/>
+      <c r="B26" s="9"/>
+      <c r="C26" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="D26" s="5"/>
       <c r="E26" s="5">
         <v>42123</v>
       </c>
       <c r="F26" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" ht="25">
+      <c r="A27" s="20"/>
+      <c r="B27" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="C27" s="8"/>
+      <c r="D27" s="8"/>
+      <c r="E27" s="11">
+        <v>42124</v>
+      </c>
+      <c r="F27" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" s="24"/>
-      <c r="B27" s="8"/>
-      <c r="C27" s="3"/>
-      <c r="D27" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="E27" s="23" t="s">
+    <row r="28" spans="1:6" ht="28">
+      <c r="A28" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="B28" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="C28" s="9"/>
+      <c r="D28" s="8"/>
+      <c r="E28" s="11">
+        <v>42125</v>
+      </c>
+      <c r="F28" s="6" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6">
+      <c r="A29" s="20"/>
+      <c r="B29" s="8"/>
+      <c r="C29" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D29" s="3"/>
+      <c r="E29" s="5">
+        <v>42130</v>
+      </c>
+      <c r="F29" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6">
+      <c r="A30" s="20"/>
+      <c r="B30" s="8"/>
+      <c r="C30" s="3"/>
+      <c r="D30" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E30" s="24" t="s">
         <v>57</v>
       </c>
-      <c r="F27" s="2" t="s">
+      <c r="F30" s="2" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" s="24"/>
-      <c r="B28" s="9"/>
-      <c r="C28" s="9" t="s">
-        <v>49</v>
-      </c>
-      <c r="D28" s="5"/>
-      <c r="E28" s="5">
-        <v>42123</v>
-      </c>
-      <c r="F28" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" s="24"/>
-      <c r="B29" s="9"/>
-      <c r="C29" s="9" t="s">
-        <v>50</v>
-      </c>
-      <c r="D29" s="5"/>
-      <c r="E29" s="5">
-        <v>42123</v>
-      </c>
-      <c r="F29" s="2" t="s">
+    <row r="31" spans="1:6" ht="37">
+      <c r="A31" s="20"/>
+      <c r="B31" s="8"/>
+      <c r="C31" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="D31" s="8"/>
+      <c r="E31" s="5">
+        <v>42131</v>
+      </c>
+      <c r="F31" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="30" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A30" s="24"/>
-      <c r="B30" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="C30" s="8"/>
-      <c r="D30" s="8"/>
-      <c r="E30" s="11">
-        <v>42124</v>
-      </c>
-      <c r="F30" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A31" s="24" t="s">
-        <v>17</v>
-      </c>
-      <c r="B31" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="C31" s="9"/>
-      <c r="D31" s="8"/>
-      <c r="E31" s="11">
-        <v>42125</v>
-      </c>
-      <c r="F31" s="6" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" s="24"/>
-      <c r="B32" s="8"/>
-      <c r="C32" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D32" s="3"/>
+    <row r="32" spans="1:6">
+      <c r="A32" s="20"/>
+      <c r="B32" s="9"/>
+      <c r="C32" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="D32" s="8"/>
       <c r="E32" s="5">
         <v>42130</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33" s="24"/>
-      <c r="B33" s="8"/>
-      <c r="C33" s="3"/>
-      <c r="D33" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="E33" s="23" t="s">
-        <v>57</v>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6">
+      <c r="A33" s="20"/>
+      <c r="B33" s="9"/>
+      <c r="C33" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="D33" s="8"/>
+      <c r="E33" s="5">
+        <v>42130</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" ht="39" x14ac:dyDescent="0.25">
-      <c r="A34" s="24"/>
-      <c r="B34" s="8"/>
-      <c r="C34" s="12" t="s">
-        <v>24</v>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6">
+      <c r="A34" s="20"/>
+      <c r="B34" s="9"/>
+      <c r="C34" s="9" t="s">
+        <v>33</v>
       </c>
       <c r="D34" s="8"/>
-      <c r="E34" s="5">
-        <v>42131</v>
+      <c r="E34" s="4">
+        <v>42137</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A35" s="24"/>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6">
+      <c r="A35" s="20"/>
       <c r="B35" s="9"/>
       <c r="C35" s="9" t="s">
-        <v>32</v>
+        <v>52</v>
       </c>
       <c r="D35" s="8"/>
-      <c r="E35" s="5">
-        <v>42130</v>
+      <c r="E35" s="4">
+        <v>42137</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A36" s="24"/>
-      <c r="B36" s="9"/>
-      <c r="C36" s="9" t="s">
-        <v>51</v>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" ht="37">
+      <c r="A36" s="20"/>
+      <c r="B36" s="8"/>
+      <c r="C36" s="12" t="s">
+        <v>24</v>
       </c>
       <c r="D36" s="8"/>
-      <c r="E36" s="5">
-        <v>42130</v>
+      <c r="E36" s="4">
+        <v>42138</v>
       </c>
       <c r="F36" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A37" s="24"/>
+    <row r="37" spans="1:6">
+      <c r="A37" s="20"/>
       <c r="B37" s="9"/>
       <c r="C37" s="9" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D37" s="8"/>
       <c r="E37" s="4">
-        <v>42137</v>
+        <v>42144</v>
       </c>
       <c r="F37" s="2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A38" s="24"/>
+    <row r="38" spans="1:6">
+      <c r="A38" s="20"/>
       <c r="B38" s="9"/>
       <c r="C38" s="9" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D38" s="8"/>
       <c r="E38" s="4">
-        <v>42137</v>
+        <v>42144</v>
       </c>
       <c r="F38" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="39" spans="1:6" ht="39" x14ac:dyDescent="0.25">
-      <c r="A39" s="24"/>
-      <c r="B39" s="8"/>
-      <c r="C39" s="12" t="s">
-        <v>24</v>
+    <row r="39" spans="1:6">
+      <c r="A39" s="20"/>
+      <c r="B39" s="9"/>
+      <c r="C39" s="9" t="s">
+        <v>54</v>
       </c>
       <c r="D39" s="8"/>
       <c r="E39" s="4">
-        <v>42138</v>
+        <v>42151</v>
       </c>
       <c r="F39" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A40" s="24"/>
-      <c r="B40" s="9"/>
+    <row r="40" spans="1:6" ht="28">
+      <c r="A40" s="20"/>
+      <c r="B40" s="8"/>
       <c r="C40" s="9" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="D40" s="8"/>
       <c r="E40" s="4">
-        <v>42144</v>
+        <v>42151</v>
       </c>
       <c r="F40" s="2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A41" s="24"/>
-      <c r="B41" s="9"/>
-      <c r="C41" s="9" t="s">
-        <v>53</v>
-      </c>
-      <c r="D41" s="8"/>
+    <row r="41" spans="1:6" ht="15" customHeight="1">
+      <c r="A41" s="20"/>
+      <c r="B41" s="8"/>
+      <c r="C41" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D41" s="1"/>
       <c r="E41" s="4">
-        <v>42144</v>
+        <v>42152</v>
       </c>
       <c r="F41" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A42" s="24"/>
-      <c r="B42" s="9"/>
-      <c r="C42" s="9" t="s">
-        <v>54</v>
-      </c>
-      <c r="D42" s="8"/>
-      <c r="E42" s="4">
-        <v>42151</v>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" ht="15" customHeight="1">
+      <c r="A42" s="20"/>
+      <c r="B42" s="8"/>
+      <c r="C42" s="1"/>
+      <c r="D42" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E42" s="23" t="s">
+        <v>57</v>
       </c>
       <c r="F42" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A43" s="24"/>
+        <v>58</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" ht="15" customHeight="1">
+      <c r="A43" s="20">
+        <v>2</v>
+      </c>
       <c r="B43" s="8"/>
-      <c r="C43" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="D43" s="8"/>
+      <c r="C43" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D43" s="1"/>
       <c r="E43" s="4">
-        <v>42151</v>
+        <v>42153</v>
       </c>
       <c r="F43" s="2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="44" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="24"/>
+    <row r="44" spans="1:6" ht="15" customHeight="1">
+      <c r="A44" s="20"/>
       <c r="B44" s="8"/>
-      <c r="C44" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D44" s="1"/>
+      <c r="C44" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="D44" s="2"/>
       <c r="E44" s="4">
-        <v>42152</v>
+        <v>42156</v>
       </c>
       <c r="F44" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="24"/>
-      <c r="B45" s="8"/>
-      <c r="C45" s="1"/>
-      <c r="D45" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="E45" s="22" t="s">
-        <v>57</v>
-      </c>
-      <c r="F45" s="2" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="24">
-        <v>2</v>
-      </c>
-      <c r="B46" s="8"/>
-      <c r="C46" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D46" s="1"/>
-      <c r="E46" s="4">
-        <v>42153</v>
-      </c>
-      <c r="F46" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="24"/>
-      <c r="B47" s="8"/>
-      <c r="C47" s="13" t="s">
-        <v>35</v>
-      </c>
-      <c r="D47" s="2"/>
-      <c r="E47" s="4">
-        <v>42156</v>
-      </c>
-      <c r="F47" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="48" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:6" ht="15" customHeight="1">
+      <c r="A45" s="16"/>
+      <c r="B45" s="17"/>
+      <c r="C45" s="17"/>
+      <c r="D45" s="18"/>
+      <c r="E45" s="14"/>
+      <c r="F45" s="18"/>
+    </row>
+    <row r="46" spans="1:6">
+      <c r="A46" s="16"/>
+      <c r="B46" s="19"/>
+      <c r="C46" s="19"/>
+      <c r="D46" s="18"/>
+      <c r="E46" s="14"/>
+      <c r="F46" s="18"/>
+    </row>
+    <row r="47" spans="1:6">
+      <c r="A47" s="16"/>
+      <c r="B47" s="18"/>
+      <c r="C47" s="18"/>
+      <c r="D47" s="19"/>
+      <c r="E47" s="14"/>
+      <c r="F47" s="18"/>
+    </row>
+    <row r="48" spans="1:6">
       <c r="A48" s="16"/>
-      <c r="B48" s="17"/>
-      <c r="C48" s="17"/>
+      <c r="B48" s="19"/>
+      <c r="C48" s="19"/>
       <c r="D48" s="18"/>
       <c r="E48" s="14"/>
       <c r="F48" s="18"/>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A49" s="16"/>
-      <c r="B49" s="19"/>
-      <c r="C49" s="19"/>
-      <c r="D49" s="18"/>
-      <c r="E49" s="14"/>
-      <c r="F49" s="18"/>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A50" s="16"/>
-      <c r="B50" s="18"/>
-      <c r="C50" s="18"/>
-      <c r="D50" s="19"/>
-      <c r="E50" s="14"/>
-      <c r="F50" s="18"/>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A51" s="16"/>
-      <c r="B51" s="19"/>
-      <c r="C51" s="19"/>
-      <c r="D51" s="18"/>
-      <c r="E51" s="14"/>
-      <c r="F51" s="18"/>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="49" spans="5:5">
+      <c r="E49" s="15"/>
+    </row>
+    <row r="50" spans="5:5">
+      <c r="E50" s="15"/>
+    </row>
+    <row r="51" spans="5:5">
+      <c r="E51" s="15"/>
+    </row>
+    <row r="52" spans="5:5">
       <c r="E52" s="15"/>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="E53" s="15"/>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="E54" s="15"/>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="E55" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="A4:A30"/>
-    <mergeCell ref="A31:A47"/>
+    <mergeCell ref="A4:A27"/>
+    <mergeCell ref="A28:A44"/>
   </mergeCells>
   <phoneticPr fontId="8" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="67" orientation="landscape" horizontalDpi="4294967293" verticalDpi="4294967293"/>
   <rowBreaks count="1" manualBreakCount="1">
-    <brk id="47" max="16383" man="1"/>
+    <brk id="44" max="16383" man="1"/>
   </rowBreaks>
   <colBreaks count="1" manualBreakCount="1">
     <brk id="7" max="1048575" man="1"/>
@@ -1775,7 +1686,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>

</xml_diff>